<commit_message>
create help text and update court label for ottawa general circ court
</commit_message>
<xml_diff>
--- a/docassemble/mlhframework/data/sources/michigan_court_info.xlsx
+++ b/docassemble/mlhframework/data/sources/michigan_court_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miadvocacyprog-my.sharepoint.com/personal/ekressmiller_lsscm_org/Documents/Attachments/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{BEB18A39-4C30-40FE-B119-921DDEE9DD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{794B3396-21CC-47BB-8216-6F3FC0CBA174}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{BEB18A39-4C30-40FE-B119-921DDEE9DD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB8E1C3A-C7B4-4E91-91E7-2EF15B32EB52}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5363,10 +5363,10 @@
     <t>Domestic</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>alternative_label</t>
+  </si>
+  <si>
+    <t>General</t>
   </si>
 </sst>
 </file>
@@ -5509,10 +5509,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5719,8 +5715,8 @@
   <dimension ref="A1:AD1002"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R4" sqref="R4"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T73" sqref="T73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5796,7 +5792,7 @@
         <v>17</v>
       </c>
       <c r="S1" s="7" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -8623,7 +8619,7 @@
       </c>
       <c r="O72" s="3"/>
       <c r="S72" s="8" t="s">
-        <v>1706</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="73" spans="1:19" ht="13" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update labels and question screen
</commit_message>
<xml_diff>
--- a/docassemble/mlhframework/data/sources/michigan_court_info.xlsx
+++ b/docassemble/mlhframework/data/sources/michigan_court_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miadvocacyprog-my.sharepoint.com/personal/ekressmiller_lsscm_org/Documents/Attachments/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{BEB18A39-4C30-40FE-B119-921DDEE9DD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB8E1C3A-C7B4-4E91-91E7-2EF15B32EB52}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{BEB18A39-4C30-40FE-B119-921DDEE9DD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBA6AE81-49A7-4CED-AFEB-873F3767A576}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5360,13 +5360,13 @@
     <t>West Olive, MI  49460</t>
   </si>
   <si>
-    <t>Domestic</t>
-  </si>
-  <si>
     <t>alternative_label</t>
   </si>
   <si>
-    <t>General</t>
+    <t>Domestic (for example: divorce, custody, child support)</t>
+  </si>
+  <si>
+    <t>General (for example: PPO, name change, foreclosure)</t>
   </si>
 </sst>
 </file>
@@ -5478,7 +5478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5493,6 +5493,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5716,7 +5719,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T73" sqref="T73"/>
+      <selection pane="bottomLeft" activeCell="S71" sqref="S71:S72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5792,7 +5795,7 @@
         <v>17</v>
       </c>
       <c r="S1" s="7" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -8574,8 +8577,8 @@
         <v>49460</v>
       </c>
       <c r="O71" s="3"/>
-      <c r="S71" s="8" t="s">
-        <v>1705</v>
+      <c r="S71" s="9" t="s">
+        <v>1706</v>
       </c>
     </row>
     <row r="72" spans="1:19" ht="13" thickBot="1" x14ac:dyDescent="0.3">
@@ -8618,7 +8621,7 @@
         <v>49417</v>
       </c>
       <c r="O72" s="3"/>
-      <c r="S72" s="8" t="s">
+      <c r="S72" s="9" t="s">
         <v>1707</v>
       </c>
     </row>

</xml_diff>